<commit_message>
Updated the time report
</commit_message>
<xml_diff>
--- a/Document/Tidsrapportering.xlsx
+++ b/Document/Tidsrapportering.xlsx
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -240,6 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +558,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,9 +628,12 @@
       <c r="D3">
         <v>0.5</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="K3" s="5">
         <f t="shared" ref="K3:K11" si="0">SUM(C3:J3)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -638,9 +642,15 @@
         <v>1</v>
       </c>
       <c r="C4" s="5"/>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
       <c r="K4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -652,9 +662,12 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
       <c r="K5" s="5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -662,7 +675,8 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5">
+      <c r="C6" s="5"/>
+      <c r="D6" s="18">
         <v>0.5</v>
       </c>
       <c r="K6" s="5">
@@ -746,11 +760,11 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
@@ -777,7 +791,7 @@
       </c>
       <c r="C15" s="16">
         <f>SUM(C12:J12)</f>
-        <v>10.5</v>
+        <v>31</v>
       </c>
       <c r="D15" s="17"/>
     </row>

</xml_diff>

<commit_message>
Updated time report, some small value changes
nothing worth noting...
</commit_message>
<xml_diff>
--- a/Document/Tidsrapportering.xlsx
+++ b/Document/Tidsrapportering.xlsx
@@ -558,7 +558,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,11 +652,11 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
@@ -797,7 +797,7 @@
       </c>
       <c r="C15" s="17">
         <f>SUM(C12:J12)</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D15" s="18"/>
     </row>

</xml_diff>

<commit_message>
Continued on victory, started on menu, updated time report
Added bitmaps for all victory conditions, wrote the procedure that
calculates victory, however this needs to be implemented in the main
loop.

Also added a bitmap for the main menu.
</commit_message>
<xml_diff>
--- a/Document/Tidsrapportering.xlsx
+++ b/Document/Tidsrapportering.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus D\Documents\GitHub\Dogfight\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Marcus D\GitHub\Dogfight\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Marcus" sheetId="4" r:id="rId1"/>
     <sheet name="Gustav" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -558,7 +558,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,11 +655,11 @@
         <v>17</v>
       </c>
       <c r="I4">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
@@ -800,7 +800,7 @@
       </c>
       <c r="C15" s="17">
         <f>SUM(C12:J12)</f>
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D15" s="18"/>
     </row>

</xml_diff>